<commit_message>
More testing and calibration
</commit_message>
<xml_diff>
--- a/12-7-15_IR-calibration.xlsx
+++ b/12-7-15_IR-calibration.xlsx
@@ -26,10 +26,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>IN</t>
+    <t>Back</t>
   </si>
   <si>
-    <t>Percent</t>
+    <t>Front</t>
   </si>
 </sst>
 </file>
@@ -45,12 +45,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,8 +71,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -99,6 +108,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>FRONT</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -228,10 +262,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>360</c:v>
+                  <c:v>893</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>1735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -261,11 +295,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="349373656"/>
-        <c:axId val="349373264"/>
+        <c:axId val="420334264"/>
+        <c:axId val="420335048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="349373656"/>
+        <c:axId val="420334264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -322,12 +356,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349373264"/>
+        <c:crossAx val="420335048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="349373264"/>
+        <c:axId val="420335048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -384,7 +418,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349373656"/>
+        <c:crossAx val="420334264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -448,6 +482,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>BACK</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -558,22 +617,22 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$6</c:f>
+              <c:f>Sheet1!$B$6:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$6</c:f>
+              <c:f>Sheet1!$C$6:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -596,11 +655,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="421394280"/>
-        <c:axId val="421402512"/>
+        <c:axId val="420333872"/>
+        <c:axId val="420332696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="421394280"/>
+        <c:axId val="420333872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,12 +716,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421402512"/>
+        <c:crossAx val="420332696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="421402512"/>
+        <c:axId val="420332696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +778,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421394280"/>
+        <c:crossAx val="420333872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1884,16 +1943,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1914,16 +1973,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>128587</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>433387</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>52387</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2208,55 +2267,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C6"/>
+  <dimension ref="B1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>360</v>
+        <v>893</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>1000</v>
+        <v>1735</v>
       </c>
       <c r="C3">
         <v>100</v>
       </c>
+      <c r="E3">
+        <v>1530</v>
+      </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>60</v>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>38</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>110</v>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>199</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>100</v>
+      </c>
+      <c r="E7">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>